<commit_message>
small fixes + modified figure output for better presentation
</commit_message>
<xml_diff>
--- a/benchmark_pingpong/results_clx16/PingPong_Limits.xlsx
+++ b/benchmark_pingpong/results_clx16/PingPong_Limits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jk869269\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\J.Klinkenberg.Local\repos\chameleon\chameleon-scripts\benchmark_pingpong\results_clx16\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -869,11 +869,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="419883192"/>
-        <c:axId val="419883584"/>
+        <c:axId val="174109840"/>
+        <c:axId val="30362544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="419883192"/>
+        <c:axId val="174109840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +977,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419883584"/>
+        <c:crossAx val="30362544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419883584"/>
+        <c:axId val="30362544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,7 +1099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="419883192"/>
+        <c:crossAx val="174109840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -1257,11 +1257,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$8</c:f>
+              <c:f>Data!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Type0_SharedMem</c:v>
+                  <c:v>Type0_DistributedMem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1477,11 +1477,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$9</c:f>
+              <c:f>Data!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Type1_SharedMem</c:v>
+                  <c:v>Type1_DistributedMem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1697,11 +1697,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$10</c:f>
+              <c:f>Data!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Type2_SharedMem</c:v>
+                  <c:v>Type2_DistributedMem</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1922,11 +1922,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="418981128"/>
-        <c:axId val="423262848"/>
+        <c:axId val="173695384"/>
+        <c:axId val="173695768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="418981128"/>
+        <c:axId val="173695384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423262848"/>
+        <c:crossAx val="173695768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2038,7 +2038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423262848"/>
+        <c:axId val="173695768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,7 +2152,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418981128"/>
+        <c:crossAx val="173695384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -3656,7 +3656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB15"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
@@ -3982,111 +3982,111 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>B3/1000</f>
+        <f t="shared" ref="B5:AB5" si="2">B3/1000</f>
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="C5">
-        <f>C3/1000</f>
+        <f t="shared" si="2"/>
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="D5">
-        <f>D3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="E5">
-        <f>E3/1000</f>
+        <f t="shared" si="2"/>
         <v>3.1999999999999999E-5</v>
       </c>
       <c r="F5">
-        <f>F3/1000</f>
+        <f t="shared" si="2"/>
         <v>6.3999999999999997E-5</v>
       </c>
       <c r="G5">
-        <f>G3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.2799999999999999E-4</v>
       </c>
       <c r="H5">
-        <f>H3/1000</f>
+        <f t="shared" si="2"/>
         <v>2.5599999999999999E-4</v>
       </c>
       <c r="I5">
-        <f>I3/1000</f>
+        <f t="shared" si="2"/>
         <v>5.1199999999999998E-4</v>
       </c>
       <c r="J5">
-        <f>J3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.024E-3</v>
       </c>
       <c r="K5">
-        <f>K3/1000</f>
+        <f t="shared" si="2"/>
         <v>2.0479999999999999E-3</v>
       </c>
       <c r="L5">
-        <f>L3/1000</f>
+        <f t="shared" si="2"/>
         <v>4.0959999999999998E-3</v>
       </c>
       <c r="M5">
-        <f>M3/1000</f>
+        <f t="shared" si="2"/>
         <v>8.1919999999999996E-3</v>
       </c>
       <c r="N5">
-        <f>N3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.6383999999999999E-2</v>
       </c>
       <c r="O5">
-        <f>O3/1000</f>
+        <f t="shared" si="2"/>
         <v>3.2767999999999999E-2</v>
       </c>
       <c r="P5">
-        <f>P3/1000</f>
+        <f t="shared" si="2"/>
         <v>6.5535999999999997E-2</v>
       </c>
       <c r="Q5">
-        <f>Q3/1000</f>
+        <f t="shared" si="2"/>
         <v>0.13107199999999999</v>
       </c>
       <c r="R5">
-        <f>R3/1000</f>
+        <f t="shared" si="2"/>
         <v>0.26214399999999999</v>
       </c>
       <c r="S5">
-        <f>S3/1000</f>
+        <f t="shared" si="2"/>
         <v>0.52428799999999998</v>
       </c>
       <c r="T5">
-        <f>T3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.048576</v>
       </c>
       <c r="U5">
-        <f>U3/1000</f>
+        <f t="shared" si="2"/>
         <v>2.0971519999999999</v>
       </c>
       <c r="V5">
-        <f>V3/1000</f>
+        <f t="shared" si="2"/>
         <v>4.1943039999999998</v>
       </c>
       <c r="W5">
-        <f>W3/1000</f>
+        <f t="shared" si="2"/>
         <v>8.3886079999999996</v>
       </c>
       <c r="X5">
-        <f>X3/1000</f>
+        <f t="shared" si="2"/>
         <v>16.777215999999999</v>
       </c>
       <c r="Y5">
-        <f>Y3/1000</f>
+        <f t="shared" si="2"/>
         <v>33.554431999999998</v>
       </c>
       <c r="Z5">
-        <f>Z3/1000</f>
+        <f t="shared" si="2"/>
         <v>67.108863999999997</v>
       </c>
       <c r="AA5">
-        <f>AA3/1000</f>
+        <f t="shared" si="2"/>
         <v>134.21772799999999</v>
       </c>
       <c r="AB5">
-        <f>AB3/1000</f>
+        <f t="shared" si="2"/>
         <v>268.43545599999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added type 2 runs
</commit_message>
<xml_diff>
--- a/benchmark_pingpong/results_clx16/PingPong_Limits.xlsx
+++ b/benchmark_pingpong/results_clx16/PingPong_Limits.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>MsgSize (Bytes)</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>MsgSize (KB) - trimmed</t>
+  </si>
+  <si>
+    <t>Mid_0_1_SharedMem</t>
+  </si>
+  <si>
+    <t>Mid_0_1_DistributedMem</t>
   </si>
 </sst>
 </file>
@@ -859,6 +865,136 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mid_0_1_SharedMem</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$B$11:$AB$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>4.8704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0745</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.359000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.130499999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137.6645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>275.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>513.52599999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>834.46600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1382.2494999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2122.3980000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2807.7614999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3380.3969999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3808.9059999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5034.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6491.5275000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6352.3670000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6571.6885000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6876.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6646.7819999999992</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6623.1299999999992</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6370.5844999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4264.5034999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3516.5495000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3457.1075000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3584.277</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3585.0639999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -869,11 +1005,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174109840"/>
-        <c:axId val="30362544"/>
+        <c:axId val="162277248"/>
+        <c:axId val="162364440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174109840"/>
+        <c:axId val="162277248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +1113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30362544"/>
+        <c:crossAx val="162364440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +1121,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30362544"/>
+        <c:axId val="162364440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,7 +1235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174109840"/>
+        <c:crossAx val="162277248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -1257,7 +1393,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$13</c:f>
+              <c:f>Data!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1382,7 +1518,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$13:$AB$13</c:f>
+              <c:f>Data!$B$14:$AB$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -1477,7 +1613,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$14</c:f>
+              <c:f>Data!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1602,7 +1738,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$14:$AB$14</c:f>
+              <c:f>Data!$B$15:$AB$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -1697,7 +1833,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$15</c:f>
+              <c:f>Data!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1822,7 +1958,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$15:$AB$15</c:f>
+              <c:f>Data!$B$16:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
@@ -1906,6 +2042,136 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1198.624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mid_0_1_DistributedMem</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$B$17:$AB$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>2.5055000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9994999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.372</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.354500000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.91749999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>135.03700000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>272.5095</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>490.084</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>868.79050000000007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1495.9825000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2132.2835</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2087.9634999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3297.3074999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3099.0754999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3564.0545000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4683.75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5455.6804999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5966.57</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10029.861499999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10800.932499999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11065.592499999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11423.415499999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11449.484</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11579.484499999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12108.8025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11922.595000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,11 +2188,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="173695384"/>
-        <c:axId val="173695768"/>
+        <c:axId val="162901504"/>
+        <c:axId val="163390224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173695384"/>
+        <c:axId val="162901504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173695768"/>
+        <c:crossAx val="163390224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2038,7 +2304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173695768"/>
+        <c:axId val="163390224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2152,7 +2418,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173695384"/>
+        <c:crossAx val="162901504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -3368,7 +3634,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9286875" cy="6024563"/>
+    <xdr:ext cx="9311173" cy="6045459"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -3654,10 +3920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AB15"/>
+  <dimension ref="A2:AB17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4353,267 +4619,493 @@
         <v>3746.6570000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B8:B9)/2</f>
+        <v>4.8704999999999998</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:AB11" si="3">SUM(C8:C9)/2</f>
+        <v>11.0745</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>21.359000000000002</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>45.53</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>85.130499999999998</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>137.6645</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>275.64999999999998</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>513.52599999999995</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>834.46600000000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>1382.2494999999999</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>2122.3980000000001</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>2807.7614999999996</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>3380.3969999999999</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>3808.9059999999999</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>5034.49</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>6491.5275000000001</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>6352.3670000000002</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>6571.6885000000002</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>6876.1</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="3"/>
+        <v>6646.7819999999992</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="3"/>
+        <v>6623.1299999999992</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="3"/>
+        <v>6370.5844999999999</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="3"/>
+        <v>4264.5034999999998</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="3"/>
+        <v>3516.5495000000001</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="3"/>
+        <v>3457.1075000000001</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="3"/>
+        <v>3584.277</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="3"/>
+        <v>3585.0639999999999</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>2.556</v>
-      </c>
-      <c r="C13">
-        <v>5.194</v>
-      </c>
-      <c r="D13">
-        <v>7.5149999999999997</v>
-      </c>
-      <c r="E13">
-        <v>18.824000000000002</v>
-      </c>
-      <c r="F13">
-        <v>30.556000000000001</v>
-      </c>
-      <c r="G13">
-        <v>69.722999999999999</v>
-      </c>
-      <c r="H13">
-        <v>128.97800000000001</v>
-      </c>
-      <c r="I13">
-        <v>259.82900000000001</v>
-      </c>
-      <c r="J13">
-        <v>484.21300000000002</v>
-      </c>
-      <c r="K13">
-        <v>827.14800000000002</v>
-      </c>
-      <c r="L13">
-        <v>1455.3040000000001</v>
-      </c>
-      <c r="M13">
-        <v>2187.8220000000001</v>
-      </c>
-      <c r="N13">
-        <v>2255.3159999999998</v>
-      </c>
-      <c r="O13">
-        <v>3513.7150000000001</v>
-      </c>
-      <c r="P13">
-        <v>4015.4540000000002</v>
-      </c>
-      <c r="Q13">
-        <v>5813.8310000000001</v>
-      </c>
-      <c r="R13">
-        <v>7970.3630000000003</v>
-      </c>
-      <c r="S13">
-        <v>9577.8359999999993</v>
-      </c>
-      <c r="T13">
-        <v>10591.066999999999</v>
-      </c>
-      <c r="U13">
-        <v>11480.303</v>
-      </c>
-      <c r="V13">
-        <v>11768.884</v>
-      </c>
-      <c r="W13">
-        <v>12030.819</v>
-      </c>
-      <c r="X13">
-        <v>12060.646000000001</v>
-      </c>
-      <c r="Y13">
-        <v>11964.198</v>
-      </c>
-      <c r="Z13">
-        <v>11837.052</v>
-      </c>
-      <c r="AA13">
-        <v>12087.288</v>
-      </c>
-      <c r="AB13">
-        <v>11669.877</v>
+      <c r="A13" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>2.4550000000000001</v>
+        <v>2.556</v>
       </c>
       <c r="C14">
-        <v>4.5469999999999997</v>
+        <v>5.194</v>
       </c>
       <c r="D14">
-        <v>8.484</v>
+        <v>7.5149999999999997</v>
       </c>
       <c r="E14">
-        <v>17.920000000000002</v>
+        <v>18.824000000000002</v>
       </c>
       <c r="F14">
-        <v>36.152999999999999</v>
+        <v>30.556000000000001</v>
       </c>
       <c r="G14">
-        <v>72.111999999999995</v>
+        <v>69.722999999999999</v>
       </c>
       <c r="H14">
-        <v>141.096</v>
+        <v>128.97800000000001</v>
       </c>
       <c r="I14">
-        <v>285.19</v>
+        <v>259.82900000000001</v>
       </c>
       <c r="J14">
-        <v>495.95499999999998</v>
+        <v>484.21300000000002</v>
       </c>
       <c r="K14">
-        <v>910.43299999999999</v>
+        <v>827.14800000000002</v>
       </c>
       <c r="L14">
-        <v>1536.6610000000001</v>
+        <v>1455.3040000000001</v>
       </c>
       <c r="M14">
-        <v>2076.7449999999999</v>
+        <v>2187.8220000000001</v>
       </c>
       <c r="N14">
-        <v>1920.6110000000001</v>
+        <v>2255.3159999999998</v>
       </c>
       <c r="O14">
-        <v>3080.9</v>
+        <v>3513.7150000000001</v>
       </c>
       <c r="P14">
-        <v>2182.6970000000001</v>
+        <v>4015.4540000000002</v>
       </c>
       <c r="Q14">
-        <v>1314.278</v>
+        <v>5813.8310000000001</v>
       </c>
       <c r="R14">
-        <v>1397.1369999999999</v>
+        <v>7970.3630000000003</v>
       </c>
       <c r="S14">
-        <v>1333.5250000000001</v>
+        <v>9577.8359999999993</v>
       </c>
       <c r="T14">
-        <v>1342.0730000000001</v>
+        <v>10591.066999999999</v>
       </c>
       <c r="U14">
-        <v>8579.42</v>
+        <v>11480.303</v>
       </c>
       <c r="V14">
-        <v>9832.9809999999998</v>
+        <v>11768.884</v>
       </c>
       <c r="W14">
-        <v>10100.366</v>
+        <v>12030.819</v>
       </c>
       <c r="X14">
-        <v>10786.184999999999</v>
+        <v>12060.646000000001</v>
       </c>
       <c r="Y14">
-        <v>10934.77</v>
+        <v>11964.198</v>
       </c>
       <c r="Z14">
-        <v>11321.916999999999</v>
+        <v>11837.052</v>
       </c>
       <c r="AA14">
-        <v>12130.316999999999</v>
+        <v>12087.288</v>
       </c>
       <c r="AB14">
-        <v>12175.313</v>
+        <v>11669.877</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="C15">
+        <v>4.5469999999999997</v>
+      </c>
+      <c r="D15">
+        <v>8.484</v>
+      </c>
+      <c r="E15">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="F15">
+        <v>36.152999999999999</v>
+      </c>
+      <c r="G15">
+        <v>72.111999999999995</v>
+      </c>
+      <c r="H15">
+        <v>141.096</v>
+      </c>
+      <c r="I15">
+        <v>285.19</v>
+      </c>
+      <c r="J15">
+        <v>495.95499999999998</v>
+      </c>
+      <c r="K15">
+        <v>910.43299999999999</v>
+      </c>
+      <c r="L15">
+        <v>1536.6610000000001</v>
+      </c>
+      <c r="M15">
+        <v>2076.7449999999999</v>
+      </c>
+      <c r="N15">
+        <v>1920.6110000000001</v>
+      </c>
+      <c r="O15">
+        <v>3080.9</v>
+      </c>
+      <c r="P15">
+        <v>2182.6970000000001</v>
+      </c>
+      <c r="Q15">
+        <v>1314.278</v>
+      </c>
+      <c r="R15">
+        <v>1397.1369999999999</v>
+      </c>
+      <c r="S15">
+        <v>1333.5250000000001</v>
+      </c>
+      <c r="T15">
+        <v>1342.0730000000001</v>
+      </c>
+      <c r="U15">
+        <v>8579.42</v>
+      </c>
+      <c r="V15">
+        <v>9832.9809999999998</v>
+      </c>
+      <c r="W15">
+        <v>10100.366</v>
+      </c>
+      <c r="X15">
+        <v>10786.184999999999</v>
+      </c>
+      <c r="Y15">
+        <v>10934.77</v>
+      </c>
+      <c r="Z15">
+        <v>11321.916999999999</v>
+      </c>
+      <c r="AA15">
+        <v>12130.316999999999</v>
+      </c>
+      <c r="AB15">
+        <v>12175.313</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1.8959999999999999</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>3.8170000000000002</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>6.9690000000000003</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>13.974</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>29.908999999999999</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>61.673999999999999</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>122.224</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>200.32499999999999</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>401.58600000000001</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>702.36599999999999</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>1206.451</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>1757.981</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <v>1634.4269999999999</v>
       </c>
-      <c r="O15">
+      <c r="O16">
         <v>2343.7750000000001</v>
       </c>
-      <c r="P15">
+      <c r="P16">
         <v>2510.5300000000002</v>
       </c>
-      <c r="Q15">
+      <c r="Q16">
         <v>3169.8090000000002</v>
       </c>
-      <c r="R15">
+      <c r="R16">
         <v>3554.9540000000002</v>
       </c>
-      <c r="S15">
+      <c r="S16">
         <v>3937.8670000000002</v>
       </c>
-      <c r="T15">
+      <c r="T16">
         <v>4197.991</v>
       </c>
-      <c r="U15">
+      <c r="U16">
         <v>4331.6959999999999</v>
       </c>
-      <c r="V15">
+      <c r="V16">
         <v>4397.8819999999996</v>
       </c>
-      <c r="W15">
+      <c r="W16">
         <v>4135.7330000000002</v>
       </c>
-      <c r="X15">
+      <c r="X16">
         <v>2417.5250000000001</v>
       </c>
-      <c r="Y15">
+      <c r="Y16">
         <v>1130.2370000000001</v>
       </c>
-      <c r="Z15">
+      <c r="Z16">
         <v>1212.9169999999999</v>
       </c>
-      <c r="AA15">
+      <c r="AA16">
         <v>1227.5740000000001</v>
       </c>
-      <c r="AB15">
+      <c r="AB16">
         <v>1198.624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B14:B15)/2</f>
+        <v>2.5055000000000001</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:AB17" si="4">SUM(C14:C15)/2</f>
+        <v>4.8704999999999998</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>7.9994999999999994</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>18.372</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>33.354500000000002</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>70.91749999999999</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>135.03700000000001</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>272.5095</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>490.084</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>868.79050000000007</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="4"/>
+        <v>1495.9825000000001</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>2132.2835</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>2087.9634999999998</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="4"/>
+        <v>3297.3074999999999</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>3099.0754999999999</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="4"/>
+        <v>3564.0545000000002</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="4"/>
+        <v>4683.75</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="4"/>
+        <v>5455.6804999999995</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="4"/>
+        <v>5966.57</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="4"/>
+        <v>10029.861499999999</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="4"/>
+        <v>10800.932499999999</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="4"/>
+        <v>11065.592499999999</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="4"/>
+        <v>11423.415499999999</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="4"/>
+        <v>11449.484</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="4"/>
+        <v>11579.484499999999</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="4"/>
+        <v>12108.8025</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="4"/>
+        <v>11922.595000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>